<commit_message>
fin version 1 base AL
</commit_message>
<xml_diff>
--- a/analisis/data/bolivia/TG YPFB.xlsx
+++ b/analisis/data/bolivia/TG YPFB.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="582">
   <si>
     <t>Utilidad Año corriente</t>
   </si>
@@ -1931,6 +1931,12 @@
   </si>
   <si>
     <t>% a partir de M$</t>
+  </si>
+  <si>
+    <t>Renta/Plusvalía</t>
+  </si>
+  <si>
+    <t>Plusvalía total</t>
   </si>
 </sst>
 </file>
@@ -2592,7 +2598,7 @@
     <xf numFmtId="167" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="241">
+  <cellXfs count="242">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -3101,6 +3107,7 @@
     <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -29098,22 +29105,22 @@
       <c r="O1" s="52"/>
     </row>
     <row r="2" spans="1:17" s="54" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="239" t="s">
+      <c r="A2" s="240" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="239"/>
-      <c r="C2" s="239"/>
-      <c r="D2" s="239"/>
-      <c r="E2" s="239"/>
-      <c r="F2" s="239"/>
-      <c r="G2" s="239"/>
-      <c r="H2" s="239"/>
-      <c r="I2" s="239"/>
-      <c r="J2" s="239"/>
-      <c r="K2" s="239"/>
-      <c r="L2" s="239"/>
-      <c r="M2" s="239"/>
-      <c r="N2" s="239"/>
+      <c r="B2" s="240"/>
+      <c r="C2" s="240"/>
+      <c r="D2" s="240"/>
+      <c r="E2" s="240"/>
+      <c r="F2" s="240"/>
+      <c r="G2" s="240"/>
+      <c r="H2" s="240"/>
+      <c r="I2" s="240"/>
+      <c r="J2" s="240"/>
+      <c r="K2" s="240"/>
+      <c r="L2" s="240"/>
+      <c r="M2" s="240"/>
+      <c r="N2" s="240"/>
     </row>
     <row r="3" spans="1:17" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="55"/>
@@ -43336,13 +43343,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD43"/>
+  <dimension ref="A1:BF43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="AP15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="AP18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AW21" sqref="AW21"/>
+      <selection pane="bottomRight" activeCell="AW30" sqref="AW30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43368,15 +43375,15 @@
     <col min="45" max="45" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:58" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="225" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="2" spans="1:56" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:58" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="225"/>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B3" s="223" t="s">
         <v>479</v>
       </c>
@@ -43440,19 +43447,25 @@
       <c r="AU3" s="223" t="s">
         <v>576</v>
       </c>
-      <c r="AW3" s="223" t="s">
+      <c r="AV3" s="223" t="s">
+        <v>581</v>
+      </c>
+      <c r="AX3" s="223" t="s">
         <v>578</v>
       </c>
       <c r="AY3" s="223" t="s">
+        <v>580</v>
+      </c>
+      <c r="BA3" s="223" t="s">
         <v>503</v>
       </c>
-      <c r="AZ3" s="223"/>
-      <c r="BC3" s="223" t="s">
+      <c r="BB3" s="223"/>
+      <c r="BE3" s="223" t="s">
         <v>503</v>
       </c>
-      <c r="BD3" s="223"/>
-    </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="BF3" s="223"/>
+    </row>
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="B4" s="222" t="s">
         <v>480</v>
       </c>
@@ -43537,23 +43550,29 @@
       <c r="AU4" s="222" t="s">
         <v>480</v>
       </c>
-      <c r="AW4" s="222" t="s">
+      <c r="AV4" s="222" t="s">
         <v>480</v>
       </c>
+      <c r="AX4" s="222" t="s">
+        <v>480</v>
+      </c>
       <c r="AY4" s="222" t="s">
+        <v>480</v>
+      </c>
+      <c r="BA4" s="222" t="s">
         <v>469</v>
       </c>
-      <c r="AZ4" s="222" t="s">
+      <c r="BB4" s="222" t="s">
         <v>470</v>
       </c>
-      <c r="BC4" s="222" t="s">
+      <c r="BE4" s="222" t="s">
         <v>469</v>
       </c>
-      <c r="BD4" s="222" t="s">
+      <c r="BF4" s="222" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="5" spans="1:56" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>487</v>
       </c>
@@ -43632,23 +43651,29 @@
       <c r="AU5" t="s">
         <v>577</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AV5" t="s">
+        <v>577</v>
+      </c>
+      <c r="AX5" t="s">
         <v>579</v>
       </c>
       <c r="AY5" t="s">
+        <v>579</v>
+      </c>
+      <c r="BA5" t="s">
         <v>573</v>
       </c>
-      <c r="AZ5" t="s">
+      <c r="BB5" t="s">
         <v>573</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BE5" t="s">
         <v>575</v>
       </c>
-      <c r="BD5" t="s">
+      <c r="BF5" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1992</v>
       </c>
@@ -43681,7 +43706,7 @@
         <v>22014.006000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1993</v>
       </c>
@@ -43714,7 +43739,7 @@
         <v>24458.969000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1994</v>
       </c>
@@ -43747,7 +43772,7 @@
         <v>27636.342000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1995</v>
       </c>
@@ -43780,7 +43805,7 @@
         <v>32235.073</v>
       </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1996</v>
       </c>
@@ -43813,7 +43838,7 @@
         <v>37536.646999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1997</v>
       </c>
@@ -43846,7 +43871,7 @@
         <v>41643.866000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1998</v>
       </c>
@@ -43879,7 +43904,7 @@
         <v>46822.326000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1999</v>
       </c>
@@ -43917,7 +43942,7 @@
         <v>48156.175000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2000</v>
       </c>
@@ -43961,8 +43986,11 @@
       <c r="AU14" s="234">
         <v>51928.491999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AV14" s="239">
+        <v>22382.432915091456</v>
+      </c>
+    </row>
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2001</v>
       </c>
@@ -44006,8 +44034,11 @@
       <c r="AU15" s="234">
         <v>53790.326999999997</v>
       </c>
-    </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AV15" s="239">
+        <v>26119.832896991178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2002</v>
       </c>
@@ -44051,8 +44082,11 @@
       <c r="AU16" s="234">
         <v>56682.328000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AV16" s="239">
+        <v>24285.879247959499</v>
+      </c>
+    </row>
+    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2003</v>
       </c>
@@ -44117,8 +44151,11 @@
       <c r="AU17" s="234">
         <v>61904.449000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AV17" s="239">
+        <v>16536.812663795921</v>
+      </c>
+    </row>
+    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2004</v>
       </c>
@@ -44183,8 +44220,11 @@
       <c r="AU18" s="234">
         <v>69626.112999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AV18" s="239">
+        <v>25195.016739419523</v>
+      </c>
+    </row>
+    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2005</v>
       </c>
@@ -44252,8 +44292,11 @@
       <c r="AU19" s="234">
         <v>77023.816999999995</v>
       </c>
-    </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AV19" s="239">
+        <v>33099.573002917045</v>
+      </c>
+    </row>
+    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2006</v>
       </c>
@@ -44323,10 +44366,13 @@
       <c r="AU20" s="234">
         <v>91747.794999999998</v>
       </c>
-      <c r="BC20" s="199"/>
-      <c r="BD20" s="199"/>
-    </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AV20" s="239">
+        <v>42562.254638684739</v>
+      </c>
+      <c r="BE20" s="199"/>
+      <c r="BF20" s="199"/>
+    </row>
+    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2007</v>
       </c>
@@ -44442,30 +44488,37 @@
       <c r="AU21" s="234">
         <v>103009.182</v>
       </c>
-      <c r="AV21" s="47"/>
-      <c r="AW21" s="199">
+      <c r="AV21" s="239">
+        <v>46614.242710020786</v>
+      </c>
+      <c r="AW21" s="47"/>
+      <c r="AX21" s="199">
         <f>AR21/AU21</f>
         <v>0.22437827516339093</v>
       </c>
-      <c r="AX21" s="47"/>
-      <c r="AY21" s="2">
-        <f t="shared" ref="AY21:AY28" si="7">AL21/AR21</f>
+      <c r="AY21" s="199">
+        <f>AR21/AV21</f>
+        <v>0.49583606295899657</v>
+      </c>
+      <c r="AZ21" s="47"/>
+      <c r="BA21" s="2">
+        <f t="shared" ref="BA21:BA28" si="7">AL21/AR21</f>
         <v>9.1681165911268556E-2</v>
       </c>
-      <c r="AZ21" s="2">
-        <f t="shared" ref="AZ21:AZ28" si="8">AM21/AR21</f>
+      <c r="BB21" s="2">
+        <f t="shared" ref="BB21:BB28" si="8">AM21/AR21</f>
         <v>0.45080237933082784</v>
       </c>
-      <c r="BC21" s="2">
+      <c r="BE21" s="2">
         <f>AO21/AS21</f>
         <v>9.1681165911268556E-2</v>
       </c>
-      <c r="BD21" s="2">
+      <c r="BF21" s="2">
         <f>AP21/AS21</f>
         <v>0.45080237933082784</v>
       </c>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2008</v>
       </c>
@@ -44581,30 +44634,37 @@
       <c r="AU22" s="234">
         <v>120693.764</v>
       </c>
-      <c r="AV22" s="47"/>
-      <c r="AW22" s="199">
-        <f t="shared" ref="AW22:AW31" si="21">AR22/AU22</f>
+      <c r="AV22" s="239">
+        <v>52494.646149859254</v>
+      </c>
+      <c r="AW22" s="47"/>
+      <c r="AX22" s="199">
+        <f t="shared" ref="AX22:AX31" si="21">AR22/AU22</f>
         <v>0.37661801951988405</v>
       </c>
-      <c r="AX22" s="47"/>
-      <c r="AY22" s="2">
+      <c r="AY22" s="199">
+        <f t="shared" ref="AY22:AY31" si="22">AR22/AV22</f>
+        <v>0.8659063295010353</v>
+      </c>
+      <c r="AZ22" s="47"/>
+      <c r="BA22" s="2">
         <f t="shared" si="7"/>
         <v>4.4011784005611392E-2</v>
       </c>
-      <c r="AZ22" s="2">
+      <c r="BB22" s="2">
         <f t="shared" si="8"/>
         <v>0.39644236337493238</v>
       </c>
-      <c r="BC22" s="2">
-        <f t="shared" ref="BC22:BC27" si="22">AO22/AS22</f>
+      <c r="BE22" s="2">
+        <f t="shared" ref="BE22:BE27" si="23">AO22/AS22</f>
         <v>4.4011784005611385E-2</v>
       </c>
-      <c r="BD22" s="2">
-        <f t="shared" ref="BD22:BD27" si="23">AP22/AS22</f>
+      <c r="BF22" s="2">
+        <f t="shared" ref="BF22:BF27" si="24">AP22/AS22</f>
         <v>0.39644236337493233</v>
       </c>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2009</v>
       </c>
@@ -44720,30 +44780,37 @@
       <c r="AU23" s="234">
         <v>121726.745</v>
       </c>
-      <c r="AV23" s="47"/>
-      <c r="AW23" s="199">
+      <c r="AV23" s="239">
+        <v>44469.092363893928</v>
+      </c>
+      <c r="AW23" s="47"/>
+      <c r="AX23" s="199">
         <f t="shared" si="21"/>
         <v>0.22652572544857047</v>
       </c>
-      <c r="AX23" s="47"/>
-      <c r="AY23" s="2">
+      <c r="AY23" s="199">
+        <f t="shared" si="22"/>
+        <v>0.62007650149402804</v>
+      </c>
+      <c r="AZ23" s="47"/>
+      <c r="BA23" s="2">
         <f t="shared" si="7"/>
         <v>7.9413244896194099E-2</v>
       </c>
-      <c r="AZ23" s="2">
+      <c r="BB23" s="2">
         <f t="shared" si="8"/>
         <v>0.32216400248600396</v>
       </c>
-      <c r="BC23" s="2">
-        <f t="shared" si="22"/>
+      <c r="BE23" s="2">
+        <f t="shared" si="23"/>
         <v>7.9413244896194099E-2</v>
       </c>
-      <c r="BD23" s="2">
-        <f t="shared" si="23"/>
+      <c r="BF23" s="2">
+        <f t="shared" si="24"/>
         <v>0.32216400248600396</v>
       </c>
     </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2010</v>
       </c>
@@ -44859,30 +44926,37 @@
       <c r="AU24" s="234">
         <v>137875.568</v>
       </c>
-      <c r="AV24" s="47"/>
-      <c r="AW24" s="199">
+      <c r="AV24" s="239">
+        <v>50027.000976298601</v>
+      </c>
+      <c r="AW24" s="47"/>
+      <c r="AX24" s="199">
         <f t="shared" si="21"/>
         <v>0.30682231598185239</v>
       </c>
-      <c r="AX24" s="47"/>
-      <c r="AY24" s="2">
+      <c r="AY24" s="199">
+        <f t="shared" si="22"/>
+        <v>0.8456093762469491</v>
+      </c>
+      <c r="AZ24" s="47"/>
+      <c r="BA24" s="2">
         <f t="shared" si="7"/>
         <v>7.1501627931479447E-2</v>
       </c>
-      <c r="AZ24" s="2">
+      <c r="BB24" s="2">
         <f t="shared" si="8"/>
         <v>0.32188424074690386</v>
       </c>
-      <c r="BC24" s="2">
-        <f t="shared" si="22"/>
+      <c r="BE24" s="2">
+        <f t="shared" si="23"/>
         <v>7.1501627931479447E-2</v>
       </c>
-      <c r="BD24" s="2">
-        <f t="shared" si="23"/>
+      <c r="BF24" s="2">
+        <f t="shared" si="24"/>
         <v>0.32188424074690386</v>
       </c>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2011</v>
       </c>
@@ -44998,30 +45072,37 @@
       <c r="AU25" s="234">
         <v>166231.56299999999</v>
       </c>
-      <c r="AV25" s="47"/>
-      <c r="AW25" s="199">
+      <c r="AV25" s="239">
+        <v>70811.916929784682</v>
+      </c>
+      <c r="AW25" s="47"/>
+      <c r="AX25" s="199">
         <f t="shared" si="21"/>
         <v>0.35350665328869202</v>
       </c>
-      <c r="AX25" s="47"/>
-      <c r="AY25" s="2">
+      <c r="AY25" s="199">
+        <f t="shared" si="22"/>
+        <v>0.82985980404043058</v>
+      </c>
+      <c r="AZ25" s="47"/>
+      <c r="BA25" s="2">
         <f t="shared" si="7"/>
         <v>0.103120278841674</v>
       </c>
-      <c r="AZ25" s="2">
+      <c r="BB25" s="2">
         <f t="shared" si="8"/>
         <v>0.29448355961009659</v>
       </c>
-      <c r="BC25" s="2">
-        <f t="shared" si="22"/>
+      <c r="BE25" s="2">
+        <f t="shared" si="23"/>
         <v>0.10312027884167399</v>
       </c>
-      <c r="BD25" s="2">
-        <f t="shared" si="23"/>
+      <c r="BF25" s="2">
+        <f t="shared" si="24"/>
         <v>0.29448355961009659</v>
       </c>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2012</v>
       </c>
@@ -45137,30 +45218,37 @@
       <c r="AU26" s="234">
         <v>187153.878</v>
       </c>
-      <c r="AV26" s="47"/>
-      <c r="AW26" s="199">
+      <c r="AV26" s="239">
+        <v>82726.009233434845</v>
+      </c>
+      <c r="AW26" s="47"/>
+      <c r="AX26" s="199">
         <f t="shared" si="21"/>
         <v>0.37271550248545537</v>
       </c>
-      <c r="AX26" s="47"/>
-      <c r="AY26" s="2">
+      <c r="AY26" s="199">
+        <f t="shared" si="22"/>
+        <v>0.84320701950021193</v>
+      </c>
+      <c r="AZ26" s="47"/>
+      <c r="BA26" s="2">
         <f t="shared" si="7"/>
         <v>0.17117614906952228</v>
       </c>
-      <c r="AZ26" s="2">
+      <c r="BB26" s="2">
         <f t="shared" si="8"/>
         <v>0.31322600315128979</v>
       </c>
-      <c r="BC26" s="2">
+      <c r="BE26" s="2">
         <f>AO26/AS26</f>
         <v>0.17117614906952228</v>
       </c>
-      <c r="BD26" s="2">
-        <f t="shared" si="23"/>
+      <c r="BF26" s="2">
+        <f t="shared" si="24"/>
         <v>0.31322600315128979</v>
       </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2013</v>
       </c>
@@ -45276,30 +45364,37 @@
       <c r="AU27" s="234">
         <v>211856.03200000001</v>
       </c>
-      <c r="AV27" s="47"/>
-      <c r="AW27" s="199">
+      <c r="AV27" s="239">
+        <v>59277.910223122337</v>
+      </c>
+      <c r="AW27" s="47"/>
+      <c r="AX27" s="199">
         <f t="shared" si="21"/>
         <v>0.3900358742096785</v>
       </c>
-      <c r="AX27" s="47"/>
-      <c r="AY27" s="2">
+      <c r="AY27" s="199">
+        <f t="shared" si="22"/>
+        <v>1.3939670331948013</v>
+      </c>
+      <c r="AZ27" s="47"/>
+      <c r="BA27" s="2">
         <f t="shared" si="7"/>
         <v>0.16770449695898357</v>
       </c>
-      <c r="AZ27" s="2">
+      <c r="BB27" s="2">
         <f t="shared" si="8"/>
         <v>0.29773245305118473</v>
       </c>
-      <c r="BC27" s="2">
-        <f t="shared" si="22"/>
+      <c r="BE27" s="2">
+        <f t="shared" si="23"/>
         <v>0.16770449695898357</v>
       </c>
-      <c r="BD27" s="2">
-        <f t="shared" si="23"/>
+      <c r="BF27" s="2">
+        <f t="shared" si="24"/>
         <v>0.29773245305118479</v>
       </c>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2014</v>
       </c>
@@ -45415,30 +45510,37 @@
       <c r="AU28" s="234">
         <v>228003.65900000001</v>
       </c>
-      <c r="AV28" s="47"/>
-      <c r="AW28" s="199">
+      <c r="AV28" s="239">
+        <v>51433.457733584481</v>
+      </c>
+      <c r="AW28" s="47"/>
+      <c r="AX28" s="199">
         <f t="shared" si="21"/>
         <v>0.39436463531654248</v>
       </c>
-      <c r="AX28" s="47"/>
-      <c r="AY28" s="2">
+      <c r="AY28" s="199">
+        <f>AR28/AV28</f>
+        <v>1.7482118409795251</v>
+      </c>
+      <c r="AZ28" s="47"/>
+      <c r="BA28" s="2">
         <f t="shared" si="7"/>
         <v>0.15482360705784573</v>
       </c>
-      <c r="AZ28" s="2">
+      <c r="BB28" s="2">
         <f t="shared" si="8"/>
         <v>0.25555963843112184</v>
       </c>
-      <c r="BC28" s="2">
+      <c r="BE28" s="2">
         <f>AO28/AS28</f>
         <v>0.15482360705784573</v>
       </c>
-      <c r="BD28" s="2">
+      <c r="BF28" s="2">
         <f>AP28/AS28</f>
         <v>0.25555963843112184</v>
       </c>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2015</v>
       </c>
@@ -45517,12 +45619,19 @@
       <c r="AU29" s="234">
         <v>228031.37</v>
       </c>
-      <c r="AW29" s="199">
+      <c r="AV29" s="239">
+        <v>66279.14078832895</v>
+      </c>
+      <c r="AX29" s="199">
         <f t="shared" si="21"/>
         <v>0.21172321986247489</v>
       </c>
-    </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AY29" s="199">
+        <f t="shared" si="22"/>
+        <v>0.72842730475698725</v>
+      </c>
+    </row>
+    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2016</v>
       </c>
@@ -45601,12 +45710,19 @@
       <c r="AU30" s="234">
         <v>234533.182</v>
       </c>
-      <c r="AW30" s="199">
+      <c r="AV30" s="239">
+        <v>59782.119588600821</v>
+      </c>
+      <c r="AX30" s="199">
         <f t="shared" si="21"/>
         <v>0.10857042430362493</v>
       </c>
-    </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AY30" s="199">
+        <f t="shared" si="22"/>
+        <v>0.42593617051802579</v>
+      </c>
+    </row>
+    <row r="31" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2017</v>
       </c>
@@ -45685,12 +45801,19 @@
       <c r="AU31" s="234">
         <v>259184.717</v>
       </c>
-      <c r="AW31" s="199">
+      <c r="AV31" s="239">
+        <v>86372.005102225026</v>
+      </c>
+      <c r="AX31" s="199">
         <f t="shared" si="21"/>
         <v>0.12757328957072858</v>
       </c>
-    </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AY31" s="199">
+        <f t="shared" si="22"/>
+        <v>0.38282134257522932</v>
+      </c>
+    </row>
+    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2018</v>
       </c>
@@ -45755,9 +45878,12 @@
       <c r="AU32" s="234">
         <v>278387.647</v>
       </c>
-      <c r="AW32" s="199"/>
-    </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AV32" s="239">
+        <v>99337.087137575407</v>
+      </c>
+      <c r="AX32" s="199"/>
+    </row>
+    <row r="33" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2019</v>
       </c>
@@ -45805,7 +45931,7 @@
       </c>
       <c r="AC33" s="230"/>
     </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2020</v>
       </c>
@@ -45853,11 +45979,11 @@
       </c>
       <c r="AC34" s="230"/>
     </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:54" x14ac:dyDescent="0.25">
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:54" x14ac:dyDescent="0.25">
       <c r="E36" s="2">
         <f>D37/E37-1</f>
         <v>0.2260550023707919</v>
@@ -45865,7 +45991,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:52" s="224" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:54" s="224" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="224" t="s">
         <v>484</v>
       </c>
@@ -45878,27 +46004,27 @@
         <v>6.2064857142857148</v>
       </c>
       <c r="H37" s="229">
-        <f t="shared" ref="H37:I37" si="24">AVERAGE(H19:H32)</f>
+        <f t="shared" ref="H37:I37" si="25">AVERAGE(H19:H32)</f>
         <v>8.097434876120861</v>
       </c>
       <c r="I37" s="229">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>6.9150230604441747</v>
       </c>
       <c r="K37" s="227">
-        <f t="shared" ref="K37" si="25">D37/H37-1</f>
+        <f t="shared" ref="K37" si="26">D37/H37-1</f>
         <v>-6.0258838316431751E-2</v>
       </c>
       <c r="L37" s="227">
-        <f t="shared" ref="L37" si="26">E37/I37-1</f>
+        <f t="shared" ref="L37" si="27">E37/I37-1</f>
         <v>-0.10246348276283956</v>
       </c>
       <c r="W37" s="232">
-        <f t="shared" ref="W37:X37" si="27">AVERAGE(W21:W28)</f>
+        <f t="shared" ref="W37:X37" si="28">AVERAGE(W21:W28)</f>
         <v>1103153205.875</v>
       </c>
       <c r="X37" s="232">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>2821587824.75</v>
       </c>
       <c r="Y37" s="232"/>
@@ -45926,7 +46052,7 @@
         <v>6889.1461025766312</v>
       </c>
       <c r="AM37" s="232">
-        <f t="shared" ref="AM37" si="28">AVERAGE(AM21:AM28)</f>
+        <f t="shared" ref="AM37" si="29">AVERAGE(AM21:AM28)</f>
         <v>17209.415702721246</v>
       </c>
       <c r="AN37" s="232"/>
@@ -45937,16 +46063,16 @@
         <f>AVERAGE(AR21:AR28)</f>
         <v>54939.144615744932</v>
       </c>
-      <c r="AY37" s="233">
+      <c r="BA37" s="233">
         <f>AL37/AR37</f>
         <v>0.12539594765736997</v>
       </c>
-      <c r="AZ37" s="233">
+      <c r="BB37" s="233">
         <f>AM37/AR37</f>
         <v>0.31324506093218685</v>
       </c>
     </row>
-    <row r="38" spans="1:52" s="224" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:54" s="224" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="224" t="s">
         <v>486</v>
       </c>
@@ -45955,23 +46081,23 @@
       <c r="K38" s="227"/>
       <c r="L38" s="227"/>
     </row>
-    <row r="39" spans="1:52" s="224" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:54" s="224" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D39" s="228"/>
       <c r="E39" s="228"/>
       <c r="K39" s="227"/>
       <c r="L39" s="227"/>
     </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A40" s="224" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B41" s="218" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:54" x14ac:dyDescent="0.25">
       <c r="B43" s="218"/>
     </row>
   </sheetData>
@@ -46236,11 +46362,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B1" s="240" t="s">
+      <c r="B1" s="241" t="s">
         <v>229</v>
       </c>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="185" t="s">

</xml_diff>